<commit_message>
strategy for zoning and batteries
</commit_message>
<xml_diff>
--- a/III.2- Strategy/Strategy Matrix/matrix.xlsx
+++ b/III.2- Strategy/Strategy Matrix/matrix.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Human Resource</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Zoning</t>
   </si>
   <si>
-    <t>Fast/Slow Charging</t>
-  </si>
-  <si>
     <t>Network Expansion</t>
   </si>
   <si>
@@ -158,6 +155,27 @@
   </si>
   <si>
     <t>Actively seek collaboration and projects with local governments to expand the network</t>
+  </si>
+  <si>
+    <t>provide plug compatibility with two-wheels vehicle, especially in emerging countries</t>
+  </si>
+  <si>
+    <t>Organize campaigns to convince home building owners of their interest to deploy charging stations</t>
+  </si>
+  <si>
+    <t>Organize communication campaigns about the sufficiency of a charger at home/office for daily journeys</t>
+  </si>
+  <si>
+    <t>Offer a complete range of services and technical support for charging stations</t>
+  </si>
+  <si>
+    <t>focus in research on how to keep good performance of batteries after many charging</t>
+  </si>
+  <si>
+    <t>Evaluate the impact of Lithium resources and possibly consider the hydrogen station market</t>
+  </si>
+  <si>
+    <t>Fast-Slow Charging</t>
   </si>
 </sst>
 </file>
@@ -181,7 +199,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -325,11 +343,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -352,6 +420,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -660,14 +752,14 @@
   <dimension ref="B1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.28515625" customWidth="1"/>
+    <col min="4" max="4" width="96.140625" customWidth="1"/>
     <col min="5" max="5" width="99.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -815,68 +907,91 @@
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="19"/>
+      <c r="C15" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="19"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="15"/>
-      <c r="C15" s="5" t="s">
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="19"/>
+      <c r="C17" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="16"/>
-      <c r="D16" s="6" t="s">
+      <c r="D17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="20"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="12"/>
+      <c r="D19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="20" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="16"/>
       <c r="C20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="E20" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B14:B18"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B14:B16"/>
     <mergeCell ref="B19:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>